<commit_message>
V0.0.6 - Added color to Glossary/Decision
</commit_message>
<xml_diff>
--- a/DMNexamples/Therapy.xlsx
+++ b/DMNexamples/Therapy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82cfe7acc6d68563/Documents/PyPI/github/pyDMNrules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82cfe7acc6d68563/Documents/PyPI/github/DecisionCentral/DMNexamples/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3451BD-2D5C-48F1-AF1F-87215C9916AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" tabRatio="784" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" tabRatio="784" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Glossary" sheetId="14" r:id="rId1"/>
@@ -1430,7 +1430,7 @@
   <dimension ref="B2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -1574,7 +1574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:D8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -1975,7 +1975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>

</xml_diff>